<commit_message>
grafic analysis automatization finished
</commit_message>
<xml_diff>
--- a/latamReturns&Ratios/latamTickers.xlsx
+++ b/latamReturns&Ratios/latamTickers.xlsx
@@ -12,7 +12,7 @@
     <sheet name="incl. deslistadas" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">MAIN!$A$1:$E$72</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">MAIN!$A$1:$E$73</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="312">
   <si>
     <t xml:space="preserve">TICKER</t>
   </si>
@@ -188,6 +188,15 @@
     <t xml:space="preserve">PAM US Equity</t>
   </si>
   <si>
+    <t xml:space="preserve">LAAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAAC US Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metals and minig</t>
+  </si>
+  <si>
     <t xml:space="preserve">VIV</t>
   </si>
   <si>
@@ -387,9 +396,6 @@
   </si>
   <si>
     <t xml:space="preserve">SGML US Equity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metals and minig</t>
   </si>
   <si>
     <t xml:space="preserve">EBR</t>
@@ -1084,13 +1090,13 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23"/>
@@ -1369,7 +1375,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>54</v>
       </c>
@@ -1377,13 +1383,13 @@
         <v>55</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1394,13 +1400,13 @@
         <v>58</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,10 +1417,10 @@
         <v>61</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>62</v>
@@ -1428,30 +1434,30 @@
         <v>64</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,7 +1468,7 @@
         <v>69</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>12</v>
@@ -1479,7 +1485,7 @@
         <v>72</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>12</v>
@@ -1496,10 +1502,10 @@
         <v>75</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>76</v>
@@ -1513,58 +1519,58 @@
         <v>78</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>29</v>
@@ -1575,13 +1581,13 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>29</v>
@@ -1592,13 +1598,13 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>29</v>
@@ -1609,19 +1615,19 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,30 +1638,30 @@
         <v>93</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,27 +1672,27 @@
         <v>98</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D34" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="C35" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>99</v>
       </c>
       <c r="E35" s="0" t="s">
         <v>103</v>
@@ -1700,30 +1706,30 @@
         <v>105</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,30 +1740,30 @@
         <v>110</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1768,7 +1774,7 @@
         <v>115</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>39</v>
@@ -1785,33 +1791,33 @@
         <v>118</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>122</v>
       </c>
@@ -1819,13 +1825,13 @@
         <v>123</v>
       </c>
       <c r="C43" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1842,7 @@
         <v>125</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>47</v>
@@ -1853,7 +1859,7 @@
         <v>127</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>47</v>
@@ -1870,47 +1876,47 @@
         <v>129</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>130</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="C47" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="C48" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="D48" s="0" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1927,7 @@
         <v>137</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>29</v>
@@ -1938,30 +1944,30 @@
         <v>139</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>140</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="C51" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,30 +1978,30 @@
         <v>144</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="C53" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C53" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="D53" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,13 +2012,13 @@
         <v>149</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,81 +2029,81 @@
         <v>151</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>152</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="C56" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="C57" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="C58" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="C58" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B59" s="0" t="s">
-        <v>163</v>
-      </c>
       <c r="C59" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2108,13 +2114,13 @@
         <v>165</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,30 +2131,30 @@
         <v>167</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>168</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B62" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="C62" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2159,13 +2165,13 @@
         <v>172</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,13 +2182,13 @@
         <v>174</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>40</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,115 +2199,115 @@
         <v>176</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>177</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="C66" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="C67" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>180</v>
-      </c>
       <c r="D67" s="0" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E67" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="B68" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="B68" s="0" t="s">
-        <v>185</v>
-      </c>
       <c r="C68" s="0" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E68" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B69" s="0" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="C69" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="D69" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E69" s="0" t="s">
         <v>189</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D70" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="E70" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B71" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="C71" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E71" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E71" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,17 +2318,34 @@
         <v>199</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D72" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="B73" s="0" t="s">
         <v>201</v>
       </c>
+      <c r="C73" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>203</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E72">
+  <autoFilter ref="A1:E73">
     <filterColumn colId="2">
       <filters>
         <filter val="Argentina"/>
@@ -2334,8 +2357,8 @@
         <filter val="Uruguay"/>
       </filters>
     </filterColumn>
-    <sortState ref="A2:E72">
-      <sortCondition ref="A2:A72" customList=""/>
+    <sortState ref="A2:E73">
+      <sortCondition ref="A2:A73" customList=""/>
     </sortState>
   </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2360,7 +2383,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23"/>
@@ -2641,13 +2664,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>8</v>
@@ -2658,47 +2681,47 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>12</v>
@@ -2709,81 +2732,81 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>19</v>
@@ -2794,13 +2817,13 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>19</v>
@@ -2811,13 +2834,13 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>29</v>
@@ -2828,13 +2851,13 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>29</v>
@@ -2845,13 +2868,13 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>29</v>
@@ -2862,13 +2885,13 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>29</v>
@@ -2879,217 +2902,217 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B35" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="E35" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>47</v>
@@ -3100,13 +3123,13 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>47</v>
@@ -3117,13 +3140,13 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>47</v>
@@ -3134,47 +3157,47 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>133</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>29</v>
@@ -3185,13 +3208,13 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>29</v>
@@ -3202,30 +3225,30 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>47</v>
@@ -3236,30 +3259,30 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>19</v>
@@ -3270,13 +3293,13 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>29</v>
@@ -3287,166 +3310,166 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B57" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B62" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E62" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>39</v>
@@ -3457,30 +3480,30 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>43</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>29</v>
@@ -3491,536 +3514,536 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B67" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>180</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>39</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D70" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B70" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>191</v>
-      </c>
       <c r="E70" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>29</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>